<commit_message>
added p and l logic
</commit_message>
<xml_diff>
--- a/public/files/Manual Statement of Profit or Loss.xlsx
+++ b/public/files/Manual Statement of Profit or Loss.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\tweaking\financial-statement-extraction\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9202FF3-25B7-4523-9962-0B5CB664456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A7F44D-372D-4C3B-B959-F9C60F99AD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Particulars</t>
   </si>
@@ -79,6 +79,27 @@
   <si>
     <t>2078-79
 2021-22</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Cells after manual Correction</t>
+  </si>
+  <si>
+    <t>Cells where incorrect information were extracted or not extracted at all</t>
+  </si>
+  <si>
+    <t>* Still can't extract all the details</t>
+  </si>
+  <si>
+    <t>observation:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Sometime confuses 8 with 3 </t>
   </si>
 </sst>
 </file>
@@ -94,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,12 +147,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,36 +496,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.125" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="32.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -502,7 +536,7 @@
         <v>10468343</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -510,7 +544,7 @@
         <v>-1136455</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -518,7 +552,7 @@
         <v>9331887</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -529,18 +563,24 @@
         <v>3960895</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
         <v>-8566576</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>-3248205</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -551,7 +591,7 @@
         <v>-4717697</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -562,27 +602,29 @@
         <v>9005006</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -593,12 +635,27 @@
         <v>9005006</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -609,12 +666,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -622,15 +679,21 @@
         <v>10468343</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25">
         <v>-1136455</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -638,7 +701,7 @@
         <v>9331887</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -649,7 +712,7 @@
         <v>3960895</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -660,7 +723,7 @@
         <v>-8248205</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -671,7 +734,7 @@
         <v>-4717697</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -682,12 +745,12 @@
         <v>-9005006</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>

</xml_diff>